<commit_message>
BP Air Tickets, Add_Queue_Retry.xaml
</commit_message>
<xml_diff>
--- a/Data/Config Prod.xlsx
+++ b/Data/Config Prod.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TVLK\Sprint 3\Traveloka_DataAutomation_Performer_Email_S3\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA0BBD3-49D4-474C-A86B-41C224A8F964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545DADF6-CAAF-4B44-8848-048E9699B6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -214,6 +214,18 @@
   </si>
   <si>
     <t>RPA_Moon_Email_S3</t>
+  </si>
+  <si>
+    <t>RPA_Moon_AutoRetryMaxDay</t>
+  </si>
+  <si>
+    <t>RPA_Moon_AutoRetrySchedule</t>
+  </si>
+  <si>
+    <t>AutoRetryMaxDay</t>
+  </si>
+  <si>
+    <t>AutoRetrySchedule</t>
   </si>
 </sst>
 </file>
@@ -591,7 +603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2864,8 +2876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2952,8 +2964,22 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
add iata export & tabula path
</commit_message>
<xml_diff>
--- a/Data/Config Prod.xlsx
+++ b/Data/Config Prod.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TVLK\Sprint 3\Traveloka_DataAutomation_Performer_Email_S3\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\Sprint 4 Email\Traveloka_DataAutomation_Performer_Email_S4\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545DADF6-CAAF-4B44-8848-048E9699B6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6453AAA5-9B47-40C9-A8E3-8E4227B6AE3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -226,6 +226,18 @@
   </si>
   <si>
     <t>AutoRetrySchedule</t>
+  </si>
+  <si>
+    <t>PathTabula</t>
+  </si>
+  <si>
+    <t>[Dev] RPA_Moon_PathTabula</t>
+  </si>
+  <si>
+    <t>PathTemplateIata</t>
+  </si>
+  <si>
+    <t>Data\Template\Template_IATA.xlsx</t>
   </si>
 </sst>
 </file>
@@ -603,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -713,7 +725,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1706,6 +1725,9 @@
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <customProperties>
+    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -2869,6 +2891,9 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <customProperties>
+    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId1"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -2876,8 +2901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2980,7 +3005,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3975,5 +4007,8 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <customProperties>
+    <customPr name="EpmWorksheetKeyString_GUID" r:id="rId1"/>
+  </customProperties>
 </worksheet>
 </file>
</xml_diff>